<commit_message>
commit by chitra 21-09-2022
</commit_message>
<xml_diff>
--- a/src/main/java/Resources/HomeSearch.xlsx
+++ b/src/main/java/Resources/HomeSearch.xlsx
@@ -30,13 +30,13 @@
     <t>tshirt</t>
   </si>
   <si>
-    <t>bag</t>
-  </si>
-  <si>
-    <t>saree</t>
-  </si>
-  <si>
-    <t>kurtis</t>
+    <t>print</t>
+  </si>
+  <si>
+    <t>testcase2</t>
+  </si>
+  <si>
+    <t>testcase3</t>
   </si>
 </sst>
 </file>
@@ -368,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -385,10 +385,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -396,24 +402,13 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>